<commit_message>
buy link testcase and update
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/UserProfileSFTcs.xlsx
+++ b/src/main/resources/excels/UserProfileSFTcs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -792,7 +792,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="105.6" x14ac:dyDescent="0.25">

</xml_diff>